<commit_message>
📊 Intraday D2 output (Mer–Dom)
</commit_message>
<xml_diff>
--- a/output/intraday/riepilogo_intraday_D2_2026-01-16.xlsx
+++ b/output/intraday/riepilogo_intraday_D2_2026-01-16.xlsx
@@ -720,10 +720,10 @@
         <v>0.79</v>
       </c>
       <c r="K2" t="n">
-        <v>1.09</v>
+        <v>1.08</v>
       </c>
       <c r="L2" t="n">
-        <v>1.11</v>
+        <v>1.05</v>
       </c>
       <c r="M2" t="n">
         <v>1.35</v>
@@ -751,27 +751,27 @@
         <v>1.1</v>
       </c>
       <c r="T2" t="n">
-        <v>1.11</v>
+        <v>1.13</v>
       </c>
       <c r="U2" t="n">
-        <v>1.08</v>
+        <v>1.01</v>
       </c>
       <c r="V2" t="n">
-        <v>1.09</v>
+        <v>1.06</v>
       </c>
       <c r="W2" t="n">
         <v>0</v>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>2026-01-15 04:21:00</t>
+          <t>2026-01-15 08:00:00</t>
         </is>
       </c>
       <c r="Y2" t="n">
         <v>1.12</v>
       </c>
       <c r="Z2" t="n">
-        <v>1.07</v>
+        <v>1.05</v>
       </c>
       <c r="AA2" t="n">
         <v>528384</v>

</xml_diff>